<commit_message>
"add Item,change the way the shield is calculated, not final"
</commit_message>
<xml_diff>
--- a/StatsBasePerLevel.xlsx
+++ b/StatsBasePerLevel.xlsx
@@ -16,27 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>HP</t>
   </si>
   <si>
     <t>MP</t>
-  </si>
-  <si>
-    <t>END</t>
-  </si>
-  <si>
-    <t>POW</t>
-  </si>
-  <si>
-    <t>CHA</t>
-  </si>
-  <si>
-    <t>VEL</t>
-  </si>
-  <si>
-    <t>SHI</t>
   </si>
   <si>
     <t>EXP_Total</t>
@@ -49,6 +34,24 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>indexShield</t>
+  </si>
+  <si>
+    <t>endurance</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>chance</t>
+  </si>
+  <si>
+    <t>velocity</t>
+  </si>
+  <si>
+    <t>shield</t>
   </si>
 </sst>
 </file>
@@ -402,20 +405,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:E7"/>
+      <selection activeCell="H2" sqref="H2:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="20" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1" max="21" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -424,27 +427,29 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -454,8 +459,9 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" s="2"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -484,18 +490,22 @@
         <v>25</v>
       </c>
       <c r="H2" s="3">
-        <f>(A2+8)*(A2-1)/2*0.04+10+0.8</f>
-        <v>10.8</v>
+        <f>(A2+8)*(A2-1)/2*5+200</f>
+        <v>200</v>
       </c>
       <c r="I2" s="3">
+        <f>H2/200</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
         <f>(A2-1)*A2*(2*A2-1)/6*100</f>
         <v>0</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -524,19 +534,23 @@
         <v>30</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H31" si="6">(A3+8)*(A3-1)/2*0.04+10+0.8</f>
-        <v>11</v>
+        <f t="shared" ref="H3:H31" si="6">(A3+8)*(A3-1)/2*5+200</f>
+        <v>225</v>
       </c>
       <c r="I3" s="3">
-        <f t="shared" ref="I3:I31" si="7">(A3-1)*A3*(2*A3-1)/6*100</f>
+        <f t="shared" ref="I3:I31" si="7">H3/200</f>
+        <v>1.125</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J31" si="8">(A3-1)*A3*(2*A3-1)/6*100</f>
         <v>100</v>
       </c>
-      <c r="J3" s="3">
-        <f>I3-I2</f>
+      <c r="K3" s="3">
+        <f>J3-J2</f>
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -566,18 +580,22 @@
       </c>
       <c r="H4" s="3">
         <f t="shared" si="6"/>
-        <v>11.24</v>
+        <v>255</v>
       </c>
       <c r="I4" s="3">
         <f t="shared" si="7"/>
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="8"/>
         <v>500</v>
       </c>
-      <c r="J4" s="3">
-        <f t="shared" ref="J4:J31" si="8">I4-I3</f>
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:K31" si="9">J4-J3</f>
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -607,18 +625,22 @@
       </c>
       <c r="H5" s="3">
         <f t="shared" si="6"/>
-        <v>11.520000000000001</v>
+        <v>290</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" si="7"/>
+        <v>1.45</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="8"/>
         <v>1400</v>
       </c>
-      <c r="J5" s="3">
-        <f t="shared" si="8"/>
+      <c r="K5" s="3">
+        <f t="shared" si="9"/>
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -648,18 +670,22 @@
       </c>
       <c r="H6" s="3">
         <f t="shared" si="6"/>
-        <v>11.84</v>
+        <v>330</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" si="7"/>
+        <v>1.65</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="8"/>
         <v>3000</v>
       </c>
-      <c r="J6" s="3">
-        <f t="shared" si="8"/>
+      <c r="K6" s="3">
+        <f t="shared" si="9"/>
         <v>1600</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -689,18 +715,22 @@
       </c>
       <c r="H7" s="3">
         <f t="shared" si="6"/>
-        <v>12.200000000000001</v>
+        <v>375</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="7"/>
+        <v>1.875</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="8"/>
         <v>5500</v>
       </c>
-      <c r="J7" s="3">
-        <f t="shared" si="8"/>
+      <c r="K7" s="3">
+        <f t="shared" si="9"/>
         <v>2500</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -730,18 +760,22 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" si="6"/>
-        <v>12.600000000000001</v>
+        <v>425</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="7"/>
+        <v>2.125</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="8"/>
         <v>9100</v>
       </c>
-      <c r="J8" s="3">
-        <f t="shared" si="8"/>
+      <c r="K8" s="3">
+        <f t="shared" si="9"/>
         <v>3600</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -771,18 +805,22 @@
       </c>
       <c r="H9" s="3">
         <f t="shared" si="6"/>
-        <v>13.040000000000001</v>
+        <v>480</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="7"/>
+        <v>2.4</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="8"/>
         <v>14000</v>
       </c>
-      <c r="J9" s="3">
-        <f t="shared" si="8"/>
+      <c r="K9" s="3">
+        <f t="shared" si="9"/>
         <v>4900</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -812,18 +850,22 @@
       </c>
       <c r="H10" s="3">
         <f t="shared" si="6"/>
-        <v>13.520000000000001</v>
+        <v>540</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="7"/>
+        <v>2.7</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="8"/>
         <v>20400</v>
       </c>
-      <c r="J10" s="3">
-        <f t="shared" si="8"/>
+      <c r="K10" s="3">
+        <f t="shared" si="9"/>
         <v>6400</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -853,18 +895,22 @@
       </c>
       <c r="H11" s="3">
         <f t="shared" si="6"/>
-        <v>14.040000000000001</v>
+        <v>605</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" si="7"/>
+        <v>3.0249999999999999</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="8"/>
         <v>28500</v>
       </c>
-      <c r="J11" s="3">
-        <f t="shared" si="8"/>
+      <c r="K11" s="3">
+        <f t="shared" si="9"/>
         <v>8100</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -894,18 +940,22 @@
       </c>
       <c r="H12" s="3">
         <f t="shared" si="6"/>
-        <v>14.600000000000001</v>
+        <v>675</v>
       </c>
       <c r="I12" s="3">
         <f t="shared" si="7"/>
+        <v>3.375</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="8"/>
         <v>38500</v>
       </c>
-      <c r="J12" s="3">
-        <f t="shared" si="8"/>
+      <c r="K12" s="3">
+        <f t="shared" si="9"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -935,18 +985,22 @@
       </c>
       <c r="H13" s="3">
         <f t="shared" si="6"/>
-        <v>15.200000000000001</v>
+        <v>750</v>
       </c>
       <c r="I13" s="3">
         <f t="shared" si="7"/>
+        <v>3.75</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="8"/>
         <v>50600</v>
       </c>
-      <c r="J13" s="3">
-        <f t="shared" si="8"/>
+      <c r="K13" s="3">
+        <f t="shared" si="9"/>
         <v>12100</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -976,18 +1030,22 @@
       </c>
       <c r="H14" s="3">
         <f t="shared" si="6"/>
-        <v>15.84</v>
+        <v>830</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="7"/>
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="8"/>
         <v>65000</v>
       </c>
-      <c r="J14" s="3">
-        <f t="shared" si="8"/>
+      <c r="K14" s="3">
+        <f t="shared" si="9"/>
         <v>14400</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1017,18 +1075,22 @@
       </c>
       <c r="H15" s="3">
         <f t="shared" si="6"/>
-        <v>16.52</v>
+        <v>915</v>
       </c>
       <c r="I15" s="3">
         <f t="shared" si="7"/>
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="8"/>
         <v>81900</v>
       </c>
-      <c r="J15" s="3">
-        <f t="shared" si="8"/>
+      <c r="K15" s="3">
+        <f t="shared" si="9"/>
         <v>16900</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1058,18 +1120,22 @@
       </c>
       <c r="H16" s="3">
         <f t="shared" si="6"/>
-        <v>17.240000000000002</v>
+        <v>1005</v>
       </c>
       <c r="I16" s="3">
         <f t="shared" si="7"/>
+        <v>5.0250000000000004</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="8"/>
         <v>101500</v>
       </c>
-      <c r="J16" s="3">
-        <f t="shared" si="8"/>
+      <c r="K16" s="3">
+        <f t="shared" si="9"/>
         <v>19600</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1099,18 +1165,22 @@
       </c>
       <c r="H17" s="3">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>1100</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="8"/>
         <v>124000</v>
       </c>
-      <c r="J17" s="3">
-        <f t="shared" si="8"/>
+      <c r="K17" s="3">
+        <f t="shared" si="9"/>
         <v>22500</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1140,18 +1210,22 @@
       </c>
       <c r="H18" s="3">
         <f t="shared" si="6"/>
-        <v>18.8</v>
+        <v>1200</v>
       </c>
       <c r="I18" s="3">
         <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" si="8"/>
         <v>149600</v>
       </c>
-      <c r="J18" s="3">
-        <f t="shared" si="8"/>
+      <c r="K18" s="3">
+        <f t="shared" si="9"/>
         <v>25600</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1181,18 +1255,22 @@
       </c>
       <c r="H19" s="3">
         <f t="shared" si="6"/>
-        <v>19.64</v>
+        <v>1305</v>
       </c>
       <c r="I19" s="3">
         <f t="shared" si="7"/>
+        <v>6.5250000000000004</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="8"/>
         <v>178500</v>
       </c>
-      <c r="J19" s="3">
-        <f t="shared" si="8"/>
+      <c r="K19" s="3">
+        <f t="shared" si="9"/>
         <v>28900</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1222,18 +1300,22 @@
       </c>
       <c r="H20" s="3">
         <f t="shared" si="6"/>
-        <v>20.52</v>
+        <v>1415</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="7"/>
+        <v>7.0750000000000002</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" si="8"/>
         <v>210900</v>
       </c>
-      <c r="J20" s="3">
-        <f t="shared" si="8"/>
+      <c r="K20" s="3">
+        <f t="shared" si="9"/>
         <v>32400</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1263,18 +1345,22 @@
       </c>
       <c r="H21" s="3">
         <f t="shared" si="6"/>
-        <v>21.44</v>
+        <v>1530</v>
       </c>
       <c r="I21" s="3">
         <f t="shared" si="7"/>
+        <v>7.65</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" si="8"/>
         <v>247000</v>
       </c>
-      <c r="J21" s="3">
-        <f t="shared" si="8"/>
+      <c r="K21" s="3">
+        <f t="shared" si="9"/>
         <v>36100</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1304,18 +1390,22 @@
       </c>
       <c r="H22" s="3">
         <f t="shared" si="6"/>
-        <v>22.400000000000002</v>
+        <v>1650</v>
       </c>
       <c r="I22" s="3">
         <f t="shared" si="7"/>
+        <v>8.25</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="8"/>
         <v>287000</v>
       </c>
-      <c r="J22" s="3">
-        <f t="shared" si="8"/>
+      <c r="K22" s="3">
+        <f t="shared" si="9"/>
         <v>40000</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1345,18 +1435,22 @@
       </c>
       <c r="H23" s="3">
         <f t="shared" si="6"/>
-        <v>23.400000000000002</v>
+        <v>1775</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="7"/>
+        <v>8.875</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="8"/>
         <v>331100</v>
       </c>
-      <c r="J23" s="3">
-        <f t="shared" si="8"/>
+      <c r="K23" s="3">
+        <f t="shared" si="9"/>
         <v>44100</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1386,18 +1480,22 @@
       </c>
       <c r="H24" s="3">
         <f t="shared" si="6"/>
-        <v>24.44</v>
+        <v>1905</v>
       </c>
       <c r="I24" s="3">
         <f t="shared" si="7"/>
+        <v>9.5250000000000004</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="8"/>
         <v>379500</v>
       </c>
-      <c r="J24" s="3">
-        <f t="shared" si="8"/>
+      <c r="K24" s="3">
+        <f t="shared" si="9"/>
         <v>48400</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1427,18 +1525,22 @@
       </c>
       <c r="H25" s="3">
         <f t="shared" si="6"/>
-        <v>25.52</v>
+        <v>2040</v>
       </c>
       <c r="I25" s="3">
         <f t="shared" si="7"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="8"/>
         <v>432400</v>
       </c>
-      <c r="J25" s="3">
-        <f t="shared" si="8"/>
+      <c r="K25" s="3">
+        <f t="shared" si="9"/>
         <v>52900</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1468,18 +1570,22 @@
       </c>
       <c r="H26" s="3">
         <f t="shared" si="6"/>
-        <v>26.64</v>
+        <v>2180</v>
       </c>
       <c r="I26" s="3">
         <f t="shared" si="7"/>
+        <v>10.9</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" si="8"/>
         <v>490000</v>
       </c>
-      <c r="J26" s="3">
-        <f t="shared" si="8"/>
+      <c r="K26" s="3">
+        <f t="shared" si="9"/>
         <v>57600</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -1509,18 +1615,22 @@
       </c>
       <c r="H27" s="3">
         <f t="shared" si="6"/>
-        <v>27.8</v>
+        <v>2325</v>
       </c>
       <c r="I27" s="3">
         <f t="shared" si="7"/>
+        <v>11.625</v>
+      </c>
+      <c r="J27" s="3">
+        <f t="shared" si="8"/>
         <v>552500</v>
       </c>
-      <c r="J27" s="3">
-        <f t="shared" si="8"/>
+      <c r="K27" s="3">
+        <f t="shared" si="9"/>
         <v>62500</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1550,18 +1660,22 @@
       </c>
       <c r="H28" s="3">
         <f t="shared" si="6"/>
-        <v>29</v>
+        <v>2475</v>
       </c>
       <c r="I28" s="3">
         <f t="shared" si="7"/>
+        <v>12.375</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="8"/>
         <v>620100</v>
       </c>
-      <c r="J28" s="3">
-        <f t="shared" si="8"/>
+      <c r="K28" s="3">
+        <f t="shared" si="9"/>
         <v>67600</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1591,18 +1705,22 @@
       </c>
       <c r="H29" s="3">
         <f t="shared" si="6"/>
-        <v>30.240000000000002</v>
+        <v>2630</v>
       </c>
       <c r="I29" s="3">
         <f t="shared" si="7"/>
+        <v>13.15</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="8"/>
         <v>693000</v>
       </c>
-      <c r="J29" s="3">
-        <f t="shared" si="8"/>
+      <c r="K29" s="3">
+        <f t="shared" si="9"/>
         <v>72900</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1632,18 +1750,22 @@
       </c>
       <c r="H30" s="3">
         <f t="shared" si="6"/>
-        <v>31.52</v>
+        <v>2790</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="7"/>
+        <v>13.95</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="8"/>
         <v>771400</v>
       </c>
-      <c r="J30" s="3">
-        <f t="shared" si="8"/>
+      <c r="K30" s="3">
+        <f t="shared" si="9"/>
         <v>78400</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1673,14 +1795,18 @@
       </c>
       <c r="H31" s="3">
         <f t="shared" si="6"/>
-        <v>32.839999999999996</v>
+        <v>2955</v>
       </c>
       <c r="I31" s="3">
         <f t="shared" si="7"/>
+        <v>14.775</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="8"/>
         <v>855500</v>
       </c>
-      <c r="J31" s="3">
-        <f t="shared" si="8"/>
+      <c r="K31" s="3">
+        <f t="shared" si="9"/>
         <v>84100</v>
       </c>
     </row>

</xml_diff>